<commit_message>
Me traje la documentacion actualizada
</commit_message>
<xml_diff>
--- a/Documentacion_de_proyecto/Tabla de funciones.xlsx
+++ b/Documentacion_de_proyecto/Tabla de funciones.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="80">
   <si>
     <t>Funciones</t>
   </si>
@@ -66,9 +66,6 @@
     <t>listarListasDeReproduccionDeUsuario(nickname:string):set&lt;DtListaDeReproduccion&gt;</t>
   </si>
   <si>
-    <t>listarListasDeReproduccionEnCategoria(cat:string):set&lt;DtVideo&gt;</t>
-  </si>
-  <si>
     <t>listarListasDeReproduccionParticularesDeUsuario() :set&lt;DtListaDeReproduccion&gt;</t>
   </si>
   <si>
@@ -250,6 +247,15 @@
   </si>
   <si>
     <t>liberarMemoriaVideo():void</t>
+  </si>
+  <si>
+    <t>listarListasDeReproduccionEnCategoria(cat:string):set&lt;DtListaDeReproduccion&gt;</t>
+  </si>
+  <si>
+    <t>iniciarSesionAdministrador(idAdmin:int, pass:string):bool</t>
+  </si>
+  <si>
+    <t>iniciarSesionUsuario(nickname:string, pass:string):bool</t>
   </si>
 </sst>
 </file>
@@ -1108,12 +1114,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U45"/>
+  <dimension ref="A1:U47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A31" sqref="A31"/>
-      <selection pane="topRight" activeCell="I32" sqref="I32"/>
+      <selection pane="topRight" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1132,7 +1138,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -1140,21 +1146,21 @@
       <c r="F1" s="50"/>
       <c r="G1" s="51"/>
       <c r="H1" s="52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I1" s="53"/>
       <c r="J1" s="53"/>
       <c r="K1" s="53"/>
       <c r="L1" s="54"/>
       <c r="M1" s="55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N1" s="56"/>
       <c r="O1" s="56"/>
       <c r="P1" s="56"/>
       <c r="Q1" s="57"/>
       <c r="R1" s="58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S1" s="59"/>
       <c r="T1" s="60"/>
@@ -1163,61 +1169,61 @@
     <row r="2" spans="1:21" s="6" customFormat="1" ht="42.45" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="62"/>
       <c r="B2" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="D2" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="E2" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="F2" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="39" t="s">
+      <c r="I2" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="J2" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="K2" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="M2" s="43" t="s">
+      <c r="N2" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="N2" s="44" t="s">
+      <c r="O2" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="O2" s="44" t="s">
+      <c r="Q2" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="P2" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q2" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="R2" s="46" t="s">
+      <c r="S2" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="S2" s="47" t="s">
+      <c r="T2" s="48" t="s">
         <v>55</v>
-      </c>
-      <c r="T2" s="48" t="s">
-        <v>56</v>
       </c>
       <c r="U2" s="13"/>
     </row>
@@ -1289,7 +1295,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L5" s="18"/>
       <c r="M5" s="29"/>
@@ -1316,7 +1322,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L6" s="18"/>
       <c r="M6" s="29"/>
@@ -1345,7 +1351,7 @@
       <c r="K7" s="8"/>
       <c r="L7" s="18"/>
       <c r="M7" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
@@ -1372,7 +1378,7 @@
       <c r="K8" s="8"/>
       <c r="L8" s="18"/>
       <c r="M8" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
@@ -1551,7 +1557,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="25" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B15" s="30"/>
       <c r="C15" s="11"/>
@@ -1565,18 +1571,10 @@
       <c r="K15" s="11"/>
       <c r="L15" s="19"/>
       <c r="M15" s="30"/>
-      <c r="N15" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="O15" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="P15" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q15" s="19" t="s">
-        <v>74</v>
-      </c>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="19"/>
       <c r="R15" s="30"/>
       <c r="S15" s="11"/>
       <c r="T15" s="19"/>
@@ -1584,52 +1582,24 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B16" s="30"/>
-      <c r="C16" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>74</v>
-      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
       <c r="E16" s="11"/>
-      <c r="F16" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="H16" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="L16" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="M16" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="N16" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="O16" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="P16" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q16" s="19" t="s">
-        <v>74</v>
-      </c>
+      <c r="F16" s="11"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="19"/>
       <c r="R16" s="30"/>
       <c r="S16" s="11"/>
       <c r="T16" s="19"/>
@@ -1637,32 +1607,32 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B17" s="30"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="11" t="s">
-        <v>74</v>
-      </c>
+      <c r="F17" s="11"/>
       <c r="G17" s="19"/>
       <c r="H17" s="30"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
-      <c r="K17" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="L17" s="19" t="s">
-        <v>74</v>
-      </c>
+      <c r="K17" s="11"/>
+      <c r="L17" s="19"/>
       <c r="M17" s="30"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
+      <c r="N17" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="O17" s="11" t="s">
+        <v>73</v>
+      </c>
       <c r="P17" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q17" s="19"/>
+        <v>73</v>
+      </c>
+      <c r="Q17" s="19" t="s">
+        <v>73</v>
+      </c>
       <c r="R17" s="30"/>
       <c r="S17" s="11"/>
       <c r="T17" s="19"/>
@@ -1670,35 +1640,51 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B18" s="30"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
+      <c r="C18" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>73</v>
+      </c>
       <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="30"/>
+      <c r="F18" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="30" t="s">
+        <v>73</v>
+      </c>
       <c r="I18" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L18" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="M18" s="30"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
+        <v>73</v>
+      </c>
+      <c r="M18" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="N18" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="O18" s="11" t="s">
+        <v>73</v>
+      </c>
       <c r="P18" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q18" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R18" s="30"/>
       <c r="S18" s="11"/>
@@ -1706,71 +1692,81 @@
       <c r="U18" s="14"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A19" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="31"/>
-      <c r="S19" s="9">
-        <v>1</v>
-      </c>
-      <c r="T19" s="20">
-        <v>1</v>
-      </c>
+      <c r="A19" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="30"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G19" s="19"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="L19" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="M19" s="30"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="30"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="19"/>
       <c r="U19" s="14"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A20" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9">
-        <v>5</v>
-      </c>
-      <c r="K20" s="9">
-        <v>5</v>
-      </c>
-      <c r="L20" s="20"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="31"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="20"/>
+      <c r="A20" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="30"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="L20" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="M20" s="30"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q20" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="R20" s="30"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="19"/>
       <c r="U20" s="14"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B21" s="31"/>
-      <c r="C21" s="9">
-        <v>4</v>
-      </c>
+      <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
@@ -1782,23 +1778,21 @@
       <c r="L21" s="20"/>
       <c r="M21" s="31"/>
       <c r="N21" s="9"/>
-      <c r="O21" s="9">
-        <v>3</v>
-      </c>
-      <c r="P21" s="9">
-        <v>6</v>
-      </c>
-      <c r="Q21" s="20">
-        <v>3</v>
-      </c>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="20"/>
       <c r="R21" s="31"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="20"/>
+      <c r="S21" s="9">
+        <v>1</v>
+      </c>
+      <c r="T21" s="20">
+        <v>1</v>
+      </c>
       <c r="U21" s="14"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B22" s="31"/>
       <c r="C22" s="9"/>
@@ -1808,8 +1802,12 @@
       <c r="G22" s="20"/>
       <c r="H22" s="31"/>
       <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
+      <c r="J22" s="9">
+        <v>5</v>
+      </c>
+      <c r="K22" s="9">
+        <v>5</v>
+      </c>
       <c r="L22" s="20"/>
       <c r="M22" s="31"/>
       <c r="N22" s="9"/>
@@ -1817,18 +1815,18 @@
       <c r="P22" s="9"/>
       <c r="Q22" s="20"/>
       <c r="R22" s="31"/>
-      <c r="S22" s="9">
-        <v>3</v>
-      </c>
+      <c r="S22" s="9"/>
       <c r="T22" s="20"/>
       <c r="U22" s="14"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B23" s="31"/>
-      <c r="C23" s="9"/>
+      <c r="C23" s="9">
+        <v>4</v>
+      </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
@@ -1839,12 +1837,16 @@
       <c r="K23" s="9"/>
       <c r="L23" s="20"/>
       <c r="M23" s="31"/>
-      <c r="N23" s="9">
+      <c r="N23" s="9"/>
+      <c r="O23" s="9">
         <v>3</v>
       </c>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="20"/>
+      <c r="P23" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q23" s="20">
+        <v>3</v>
+      </c>
       <c r="R23" s="31"/>
       <c r="S23" s="9"/>
       <c r="T23" s="20"/>
@@ -1852,12 +1854,10 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" s="26" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="B24" s="31"/>
-      <c r="C24" s="9">
-        <v>6</v>
-      </c>
+      <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
@@ -1873,31 +1873,31 @@
       <c r="P24" s="9"/>
       <c r="Q24" s="20"/>
       <c r="R24" s="31"/>
-      <c r="S24" s="9"/>
+      <c r="S24" s="9">
+        <v>3</v>
+      </c>
       <c r="T24" s="20"/>
       <c r="U24" s="14"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" s="26" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B25" s="31"/>
-      <c r="C25" s="9">
-        <v>5</v>
-      </c>
+      <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
-      <c r="G25" s="20">
-        <v>3</v>
-      </c>
+      <c r="G25" s="20"/>
       <c r="H25" s="31"/>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
       <c r="L25" s="20"/>
       <c r="M25" s="31"/>
-      <c r="N25" s="9"/>
+      <c r="N25" s="9">
+        <v>3</v>
+      </c>
       <c r="O25" s="9"/>
       <c r="P25" s="9"/>
       <c r="Q25" s="20"/>
@@ -1908,54 +1908,26 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" s="26" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B26" s="31"/>
       <c r="C26" s="9">
-        <v>1</v>
-      </c>
-      <c r="D26" s="9">
-        <v>1</v>
-      </c>
-      <c r="E26" s="9">
-        <v>1</v>
-      </c>
-      <c r="F26" s="9">
-        <v>1</v>
-      </c>
-      <c r="G26" s="20">
-        <v>1</v>
-      </c>
-      <c r="H26" s="31">
-        <v>1</v>
-      </c>
-      <c r="I26" s="9">
-        <v>1</v>
-      </c>
-      <c r="J26" s="9">
-        <v>1</v>
-      </c>
-      <c r="K26" s="9">
-        <v>1</v>
-      </c>
-      <c r="L26" s="20">
-        <v>1</v>
-      </c>
-      <c r="M26" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="N26" s="9">
-        <v>1</v>
-      </c>
-      <c r="O26" s="9">
-        <v>1</v>
-      </c>
-      <c r="P26" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="20">
-        <v>1</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="20"/>
       <c r="R26" s="31"/>
       <c r="S26" s="9"/>
       <c r="T26" s="20"/>
@@ -1963,14 +1935,18 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" s="26" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B27" s="31"/>
-      <c r="C27" s="9"/>
+      <c r="C27" s="9">
+        <v>5</v>
+      </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="20"/>
+      <c r="G27" s="20">
+        <v>3</v>
+      </c>
       <c r="H27" s="31"/>
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
@@ -1978,13 +1954,9 @@
       <c r="L27" s="20"/>
       <c r="M27" s="31"/>
       <c r="N27" s="9"/>
-      <c r="O27" s="9">
-        <v>5</v>
-      </c>
+      <c r="O27" s="9"/>
       <c r="P27" s="9"/>
-      <c r="Q27" s="20">
-        <v>5</v>
-      </c>
+      <c r="Q27" s="20"/>
       <c r="R27" s="31"/>
       <c r="S27" s="9"/>
       <c r="T27" s="20"/>
@@ -1992,36 +1964,54 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" s="26" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B28" s="31"/>
       <c r="C28" s="9">
-        <v>3</v>
-      </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="31"/>
+        <v>1</v>
+      </c>
+      <c r="D28" s="9">
+        <v>1</v>
+      </c>
+      <c r="E28" s="9">
+        <v>1</v>
+      </c>
+      <c r="F28" s="9">
+        <v>1</v>
+      </c>
+      <c r="G28" s="20">
+        <v>1</v>
+      </c>
+      <c r="H28" s="31">
+        <v>1</v>
+      </c>
       <c r="I28" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J28" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K28" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L28" s="20">
-        <v>3</v>
-      </c>
-      <c r="M28" s="31"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="M28" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="N28" s="9">
+        <v>1</v>
+      </c>
+      <c r="O28" s="9">
+        <v>1</v>
+      </c>
       <c r="P28" s="9">
-        <v>3</v>
-      </c>
-      <c r="Q28" s="20"/>
+        <v>1</v>
+      </c>
+      <c r="Q28" s="20">
+        <v>1</v>
+      </c>
       <c r="R28" s="31"/>
       <c r="S28" s="9"/>
       <c r="T28" s="20"/>
@@ -2029,7 +2019,7 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" s="26" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B29" s="31"/>
       <c r="C29" s="9"/>
@@ -2044,73 +2034,85 @@
       <c r="L29" s="20"/>
       <c r="M29" s="31"/>
       <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
+      <c r="O29" s="9">
+        <v>5</v>
+      </c>
       <c r="P29" s="9"/>
-      <c r="Q29" s="20"/>
+      <c r="Q29" s="20">
+        <v>5</v>
+      </c>
       <c r="R29" s="31"/>
-      <c r="S29" s="9">
-        <v>2</v>
-      </c>
+      <c r="S29" s="9"/>
       <c r="T29" s="20"/>
       <c r="U29" s="14"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A30" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="8">
-        <v>5</v>
-      </c>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="29"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="18"/>
+      <c r="A30" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="31"/>
+      <c r="C30" s="9">
+        <v>3</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="9">
+        <v>3</v>
+      </c>
+      <c r="J30" s="9">
+        <v>3</v>
+      </c>
+      <c r="K30" s="9">
+        <v>3</v>
+      </c>
+      <c r="L30" s="20">
+        <v>3</v>
+      </c>
+      <c r="M30" s="31"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q30" s="20"/>
+      <c r="R30" s="31"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="20"/>
       <c r="U30" s="14"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A31" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8">
-        <v>4</v>
-      </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="29"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="18"/>
+      <c r="A31" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="31"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="31"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="20"/>
+      <c r="R31" s="31"/>
+      <c r="S31" s="9">
+        <v>2</v>
+      </c>
+      <c r="T31" s="20"/>
       <c r="U31" s="14"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B32" s="29"/>
       <c r="C32" s="8"/>
@@ -2119,14 +2121,14 @@
       <c r="F32" s="8"/>
       <c r="G32" s="18"/>
       <c r="H32" s="29"/>
-      <c r="I32" s="8">
-        <v>5</v>
-      </c>
+      <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
       <c r="L32" s="18"/>
       <c r="M32" s="29"/>
-      <c r="N32" s="8"/>
+      <c r="N32" s="8">
+        <v>5</v>
+      </c>
       <c r="O32" s="8"/>
       <c r="P32" s="8"/>
       <c r="Q32" s="18"/>
@@ -2136,74 +2138,74 @@
       <c r="U32" s="14"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A33" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="28"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10">
-        <v>3</v>
-      </c>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="17"/>
-      <c r="M33" s="28"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
-      <c r="P33" s="10"/>
-      <c r="Q33" s="17"/>
-      <c r="R33" s="28"/>
-      <c r="S33" s="10"/>
-      <c r="T33" s="17"/>
+      <c r="A33" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="29"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8">
+        <v>4</v>
+      </c>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="29"/>
+      <c r="S33" s="8"/>
+      <c r="T33" s="18"/>
       <c r="U33" s="14"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A34" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="17">
-        <v>7</v>
-      </c>
-      <c r="M34" s="28"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="10"/>
-      <c r="P34" s="10"/>
-      <c r="Q34" s="17"/>
-      <c r="R34" s="28"/>
-      <c r="S34" s="10"/>
-      <c r="T34" s="17"/>
+      <c r="A34" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="29"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="8">
+        <v>5</v>
+      </c>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="29"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="29"/>
+      <c r="S34" s="8"/>
+      <c r="T34" s="18"/>
       <c r="U34" s="14"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" s="23" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B35" s="28"/>
       <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
+      <c r="D35" s="10">
+        <v>3</v>
+      </c>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
       <c r="G35" s="17"/>
       <c r="H35" s="28"/>
       <c r="I35" s="10"/>
-      <c r="J35" s="10">
-        <v>6</v>
-      </c>
+      <c r="J35" s="10"/>
       <c r="K35" s="10"/>
       <c r="L35" s="17"/>
       <c r="M35" s="28"/>
@@ -2218,7 +2220,7 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" s="23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B36" s="28"/>
       <c r="C36" s="10"/>
@@ -2230,14 +2232,14 @@
       <c r="I36" s="10"/>
       <c r="J36" s="10"/>
       <c r="K36" s="10"/>
-      <c r="L36" s="17"/>
+      <c r="L36" s="17">
+        <v>7</v>
+      </c>
       <c r="M36" s="28"/>
       <c r="N36" s="10"/>
       <c r="O36" s="10"/>
       <c r="P36" s="10"/>
-      <c r="Q36" s="17">
-        <v>7</v>
-      </c>
+      <c r="Q36" s="17"/>
       <c r="R36" s="28"/>
       <c r="S36" s="10"/>
       <c r="T36" s="17"/>
@@ -2245,21 +2247,19 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" s="23" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B37" s="28"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
-      <c r="F37" s="10">
-        <v>4</v>
-      </c>
-      <c r="G37" s="17">
-        <v>4</v>
-      </c>
+      <c r="F37" s="10"/>
+      <c r="G37" s="17"/>
       <c r="H37" s="28"/>
       <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
+      <c r="J37" s="10">
+        <v>6</v>
+      </c>
       <c r="K37" s="10"/>
       <c r="L37" s="17"/>
       <c r="M37" s="28"/>
@@ -2273,119 +2273,89 @@
       <c r="U37" s="14"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A38" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" s="31"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="31"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="20"/>
-      <c r="M38" s="31"/>
-      <c r="N38" s="9">
+      <c r="A38" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="28"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="28"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="17">
+        <v>7</v>
+      </c>
+      <c r="R38" s="28"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="17"/>
+      <c r="U38" s="14"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A39" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="28"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10">
         <v>4</v>
       </c>
-      <c r="O38" s="9">
+      <c r="G39" s="17">
         <v>4</v>
       </c>
-      <c r="P38" s="9">
-        <v>7</v>
-      </c>
-      <c r="Q38" s="20">
-        <v>4</v>
-      </c>
-      <c r="R38" s="31"/>
-      <c r="S38" s="9"/>
-      <c r="T38" s="20"/>
-      <c r="U38" s="14"/>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A39" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="9">
-        <v>2</v>
-      </c>
-      <c r="D39" s="9">
-        <v>2</v>
-      </c>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9">
-        <v>3</v>
-      </c>
-      <c r="G39" s="20">
-        <v>2</v>
-      </c>
-      <c r="H39" s="31">
-        <v>2</v>
-      </c>
-      <c r="I39" s="9">
-        <v>2</v>
-      </c>
-      <c r="J39" s="9">
-        <v>2</v>
-      </c>
-      <c r="K39" s="9">
-        <v>2</v>
-      </c>
-      <c r="L39" s="20">
-        <v>2</v>
-      </c>
-      <c r="M39" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="N39" s="9">
-        <v>2</v>
-      </c>
-      <c r="O39" s="9">
-        <v>2</v>
-      </c>
-      <c r="P39" s="9">
-        <v>2</v>
-      </c>
-      <c r="Q39" s="20">
-        <v>2</v>
-      </c>
-      <c r="R39" s="31"/>
-      <c r="S39" s="9"/>
-      <c r="T39" s="20"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="28"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="17"/>
+      <c r="R39" s="28"/>
+      <c r="S39" s="10"/>
+      <c r="T39" s="17"/>
       <c r="U39" s="14"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" s="26" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B40" s="31"/>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
-      <c r="F40" s="9">
-        <v>2</v>
-      </c>
+      <c r="F40" s="9"/>
       <c r="G40" s="20"/>
       <c r="H40" s="31"/>
       <c r="I40" s="9"/>
       <c r="J40" s="9"/>
-      <c r="K40" s="9">
-        <v>6</v>
-      </c>
-      <c r="L40" s="20">
-        <v>5</v>
-      </c>
+      <c r="K40" s="9"/>
+      <c r="L40" s="20"/>
       <c r="M40" s="31"/>
-      <c r="N40" s="9"/>
-      <c r="O40" s="9"/>
+      <c r="N40" s="9">
+        <v>4</v>
+      </c>
+      <c r="O40" s="9">
+        <v>4</v>
+      </c>
       <c r="P40" s="9">
-        <v>5</v>
-      </c>
-      <c r="Q40" s="20"/>
+        <v>7</v>
+      </c>
+      <c r="Q40" s="20">
+        <v>4</v>
+      </c>
       <c r="R40" s="31"/>
       <c r="S40" s="9"/>
       <c r="T40" s="20"/>
@@ -2393,35 +2363,51 @@
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" s="26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B41" s="31"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
+      <c r="C41" s="9">
+        <v>2</v>
+      </c>
+      <c r="D41" s="9">
+        <v>2</v>
+      </c>
       <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="31"/>
+      <c r="F41" s="9">
+        <v>3</v>
+      </c>
+      <c r="G41" s="20">
+        <v>2</v>
+      </c>
+      <c r="H41" s="31">
+        <v>2</v>
+      </c>
       <c r="I41" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J41" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K41" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L41" s="20">
-        <v>4</v>
-      </c>
-      <c r="M41" s="31"/>
-      <c r="N41" s="9"/>
-      <c r="O41" s="9"/>
+        <v>2</v>
+      </c>
+      <c r="M41" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="N41" s="9">
+        <v>2</v>
+      </c>
+      <c r="O41" s="9">
+        <v>2</v>
+      </c>
       <c r="P41" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q41" s="20">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="R41" s="31"/>
       <c r="S41" s="9"/>
@@ -2429,93 +2415,163 @@
       <c r="U41" s="14"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="31"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9">
+        <v>2</v>
+      </c>
+      <c r="G42" s="20"/>
+      <c r="H42" s="31"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9">
+        <v>6</v>
+      </c>
+      <c r="L42" s="20">
+        <v>5</v>
+      </c>
+      <c r="M42" s="31"/>
+      <c r="N42" s="9"/>
+      <c r="O42" s="9"/>
+      <c r="P42" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q42" s="20"/>
+      <c r="R42" s="31"/>
+      <c r="S42" s="9"/>
+      <c r="T42" s="20"/>
+      <c r="U42" s="14"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A43" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" s="31"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="9">
+        <v>4</v>
+      </c>
+      <c r="J43" s="9">
+        <v>4</v>
+      </c>
+      <c r="K43" s="9">
+        <v>4</v>
+      </c>
+      <c r="L43" s="20">
+        <v>4</v>
+      </c>
+      <c r="M43" s="31"/>
+      <c r="N43" s="9"/>
+      <c r="O43" s="9"/>
+      <c r="P43" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q43" s="20">
+        <v>6</v>
+      </c>
+      <c r="R43" s="31"/>
+      <c r="S43" s="9"/>
+      <c r="T43" s="20"/>
+      <c r="U43" s="14"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A44" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="28"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="17"/>
+      <c r="M44" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="N44" s="10"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="17"/>
+      <c r="R44" s="28"/>
+      <c r="S44" s="10"/>
+      <c r="T44" s="17"/>
+      <c r="U44" s="14"/>
+    </row>
+    <row r="45" spans="1:21" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="28"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
-      <c r="L42" s="17"/>
-      <c r="M42" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="N42" s="10"/>
-      <c r="O42" s="10"/>
-      <c r="P42" s="10"/>
-      <c r="Q42" s="17"/>
-      <c r="R42" s="28"/>
-      <c r="S42" s="10"/>
-      <c r="T42" s="17"/>
-      <c r="U42" s="14"/>
-    </row>
-    <row r="43" spans="1:21" ht="14.55" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="32"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="32"/>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="21"/>
-      <c r="L43" s="22"/>
-      <c r="M43" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="N43" s="21"/>
-      <c r="O43" s="21"/>
-      <c r="P43" s="21"/>
-      <c r="Q43" s="22"/>
-      <c r="R43" s="32"/>
-      <c r="S43" s="21"/>
-      <c r="T43" s="22"/>
-      <c r="U43" s="14"/>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A44" s="15"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
-      <c r="I44" s="16"/>
-      <c r="J44" s="16"/>
-      <c r="K44" s="16"/>
-      <c r="L44" s="16"/>
-      <c r="M44" s="16"/>
-      <c r="N44" s="16"/>
-      <c r="O44" s="16"/>
-      <c r="P44" s="16"/>
-      <c r="Q44" s="16"/>
-      <c r="R44" s="16"/>
-      <c r="S44" s="16"/>
-      <c r="T44" s="16"/>
-    </row>
-    <row r="45" spans="1:21" ht="41.95" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C45" s="3" t="s">
+      <c r="B45" s="32"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="22"/>
+      <c r="M45" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="N45" s="21"/>
+      <c r="O45" s="21"/>
+      <c r="P45" s="21"/>
+      <c r="Q45" s="22"/>
+      <c r="R45" s="32"/>
+      <c r="S45" s="21"/>
+      <c r="T45" s="22"/>
+      <c r="U45" s="14"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A46" s="15"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16"/>
+      <c r="M46" s="16"/>
+      <c r="N46" s="16"/>
+      <c r="O46" s="16"/>
+      <c r="P46" s="16"/>
+      <c r="Q46" s="16"/>
+      <c r="R46" s="16"/>
+      <c r="S46" s="16"/>
+      <c r="T46" s="16"/>
+    </row>
+    <row r="47" spans="1:21" ht="41.95" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="O45" s="4" t="s">
-        <v>69</v>
+      <c r="O47" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>